<commit_message>
made a emailSender class instead of the old one to make it completely reuseable now, and had to add to the .ini file
</commit_message>
<xml_diff>
--- a/src/data/data_copy.xlsx
+++ b/src/data/data_copy.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,42 +558,38 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>01-02-2024</t>
+          <t>01-03-2024</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>42</v>
+        <v>42.67</v>
       </c>
       <c r="D3" t="n">
-        <v>31</v>
+        <v>32.32</v>
       </c>
       <c r="E3" t="n">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F3" t="n">
-        <v>6</v>
+        <v>8.1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Clear</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>hat</t>
-        </is>
-      </c>
+          <t>scattered clouds</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>light hoddie</t>
+          <t>heavy hoddie</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>sweat pants</t>
+          <t>joggers</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -602,44 +598,48 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>solid outfit</t>
+          <t xml:space="preserve"> None</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>01-02-2024</t>
+          <t>01-05-2024</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>42.53</v>
+        <v>36.54</v>
       </c>
       <c r="D4" t="n">
-        <v>32.74</v>
+        <v>27.82</v>
       </c>
       <c r="E4" t="n">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F4" t="n">
-        <v>9.369999999999999</v>
+        <v>10.09</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>clear sky</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>hat</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>long sleeve shirt</t>
+          <t>tshirt</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -652,116 +652,14 @@
           <t>sneakers</t>
         </is>
       </c>
-      <c r="L4" t="n">
-        <v>8</v>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>chilly</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>01-03-2024</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>42.67</v>
-      </c>
-      <c r="D5" t="n">
-        <v>32.32</v>
-      </c>
-      <c r="E5" t="n">
-        <v>55</v>
-      </c>
-      <c r="F5" t="n">
-        <v>8.1</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>scattered clouds</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>heavy hoddie</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>joggers</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>boots</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>10</v>
-      </c>
-      <c r="M5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>01-03-2024</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>42.82</v>
-      </c>
-      <c r="D6" t="n">
-        <v>32.32</v>
-      </c>
-      <c r="E6" t="n">
-        <v>55</v>
-      </c>
-      <c r="F6" t="n">
-        <v>7.56</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>scattered clouds</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>asdf</t>
+          <t>cold</t>
         </is>
       </c>
     </row>

</xml_diff>